<commit_message>
ilk wave winding tasarımı tamamlandı
</commit_message>
<xml_diff>
--- a/matlab analitik model/double_sided.xlsx
+++ b/matlab analitik model/double_sided.xlsx
@@ -1,16 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20353"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\PCB-Motor\matlab analitik model\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965667E2-A049-4987-A5DE-9FDD9D345359}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="20940" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" fullCalcOnLoad="true"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -113,22 +120,28 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -136,47 +149,360 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P102"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="true"/>
-    <col min="2" max="2" width="16" customWidth="true"/>
-    <col min="3" max="3" width="20" customWidth="true"/>
-    <col min="4" max="4" width="19.5703125" customWidth="true"/>
-    <col min="5" max="5" width="17" customWidth="true"/>
-    <col min="6" max="6" width="25.85546875" customWidth="true"/>
-    <col min="7" max="7" width="15.5703125" customWidth="true"/>
-    <col min="8" max="8" width="22.7109375" customWidth="true"/>
-    <col min="9" max="9" width="18.7109375" customWidth="true"/>
-    <col min="10" max="10" width="11.7109375" customWidth="true"/>
-    <col min="11" max="11" width="11.7109375" customWidth="true"/>
-    <col min="12" max="12" width="12.7109375" customWidth="true"/>
-    <col min="13" max="13" width="12.7109375" customWidth="true"/>
-    <col min="14" max="14" width="14.28515625" customWidth="true"/>
-    <col min="15" max="15" width="14.7109375" customWidth="true"/>
-    <col min="16" max="16" width="11.7109375" customWidth="true"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="11" width="11.7109375" customWidth="1"/>
+    <col min="12" max="13" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -226,7 +552,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -246,10 +572,10 @@
         <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>17</v>
@@ -276,7 +602,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>50</v>
       </c>
@@ -290,13 +616,13 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="F3">
         <v>1.1941438923248031</v>
       </c>
       <c r="G3">
-        <v>3.9248836349446107e-05</v>
+        <v>3.9248836349446107E-5</v>
       </c>
       <c r="H3">
         <v>37.812562550306254</v>
@@ -326,7 +652,7 @@
         <v>1.8304009898485551</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>50</v>
       </c>
@@ -334,19 +660,19 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <v>1.8999999999999999</v>
+        <v>1.9</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="F4">
         <v>1.1941438923248031</v>
       </c>
       <c r="G4">
-        <v>3.9248836349446107e-05</v>
+        <v>3.9248836349446107E-5</v>
       </c>
       <c r="H4">
         <v>39.026026852196779</v>
@@ -376,7 +702,7 @@
         <v>1.9267378840511109</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>50</v>
       </c>
@@ -390,13 +716,13 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="F5">
         <v>1.1941438923248031</v>
       </c>
       <c r="G5">
-        <v>3.9248836349446107e-05</v>
+        <v>3.9248836349446107E-5</v>
       </c>
       <c r="H5">
         <v>40.319957377706714</v>
@@ -426,7 +752,7 @@
         <v>2.0337788776095058</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>50</v>
       </c>
@@ -440,13 +766,13 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="F6">
         <v>1.1941438923248031</v>
       </c>
       <c r="G6">
-        <v>3.9248836349446107e-05</v>
+        <v>3.9248836349446107E-5</v>
       </c>
       <c r="H6">
         <v>41.70263230746869</v>
@@ -476,57 +802,57 @@
         <v>2.1534129292335944</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7">
-        <v>50</v>
-      </c>
-      <c r="B7">
-        <v>7</v>
-      </c>
-      <c r="C7">
+    <row r="7" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>50</v>
+      </c>
+      <c r="B7" s="2">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2">
         <v>2</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>2</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>4.8999999999999995</v>
       </c>
-      <c r="F7">
-        <v>1.1941438923248031</v>
-      </c>
-      <c r="G7">
-        <v>2.9436627262084583e-05</v>
-      </c>
-      <c r="H7">
+      <c r="F7" s="2">
+        <v>1.1941438923248031</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2.9436627262084583E-5</v>
+      </c>
+      <c r="H7" s="2">
         <v>44.975361600628915</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="2">
         <v>1.9521092704210978</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="2">
         <v>9.6683503588791577</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="2">
         <v>1.2422759453636116</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="2">
         <v>0.67232361276103203</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="2">
         <v>0.73046600321751864</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="2">
         <v>0.48230771197463534</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="2">
         <v>0.22369524468698243</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="2">
         <v>2.1560928246352766</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>50</v>
       </c>
@@ -534,7 +860,7 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>1.8999999999999999</v>
+        <v>1.9</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -546,7 +872,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G8">
-        <v>2.9436627262084583e-05</v>
+        <v>2.9436627262084583E-5</v>
       </c>
       <c r="H8">
         <v>46.247744304191265</v>
@@ -576,7 +902,7 @@
         <v>2.2695713943529232</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>50</v>
       </c>
@@ -584,19 +910,19 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>1.6000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="F9">
         <v>1.1941438923248031</v>
       </c>
       <c r="G9">
-        <v>3.9248836349446107e-05</v>
+        <v>3.9248836349446107E-5</v>
       </c>
       <c r="H9">
         <v>43.183505665122894</v>
@@ -626,7 +952,7 @@
         <v>2.2880012373106942</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>50</v>
       </c>
@@ -646,7 +972,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G10">
-        <v>2.9436627262084583e-05</v>
+        <v>2.9436627262084583E-5</v>
       </c>
       <c r="H10">
         <v>47.594216133263238</v>
@@ -676,7 +1002,7 @@
         <v>2.3956586940391964</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>50</v>
       </c>
@@ -690,13 +1016,13 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="F11">
         <v>1.1941438923248031</v>
       </c>
       <c r="G11">
-        <v>3.9248836349446107e-05</v>
+        <v>3.9248836349446107E-5</v>
       </c>
       <c r="H11">
         <v>44.773423776595386</v>
@@ -726,7 +1052,7 @@
         <v>2.4405346531314067</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>50</v>
       </c>
@@ -746,7 +1072,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G12">
-        <v>2.9436627262084583e-05</v>
+        <v>2.9436627262084583E-5</v>
       </c>
       <c r="H12">
         <v>49.021442305655405</v>
@@ -776,7 +1102,7 @@
         <v>2.5365797936885608</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>50</v>
       </c>
@@ -784,19 +1110,19 @@
         <v>7</v>
       </c>
       <c r="C13">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="F13">
         <v>1.1941438923248031</v>
       </c>
       <c r="G13">
-        <v>3.9248836349446107e-05</v>
+        <v>3.9248836349446107E-5</v>
       </c>
       <c r="H13">
         <v>46.48489137441252</v>
@@ -826,7 +1152,7 @@
         <v>2.6148585569265075</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>50</v>
       </c>
@@ -846,7 +1172,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G14">
-        <v>2.3549301809667665e-05</v>
+        <v>2.3549301809667665E-5</v>
       </c>
       <c r="H14">
         <v>48.006646616335786</v>
@@ -876,7 +1202,7 @@
         <v>2.6270834880840557</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>50</v>
       </c>
@@ -884,7 +1210,7 @@
         <v>7</v>
       </c>
       <c r="C15">
-        <v>1.6000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -896,7 +1222,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G15">
-        <v>2.9436627262084583e-05</v>
+        <v>2.9436627262084583E-5</v>
       </c>
       <c r="H15">
         <v>50.536912244811958</v>
@@ -926,7 +1252,7 @@
         <v>2.6951160307940958</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>50</v>
       </c>
@@ -934,7 +1260,7 @@
         <v>7</v>
       </c>
       <c r="C16">
-        <v>1.8999999999999999</v>
+        <v>1.9</v>
       </c>
       <c r="D16">
         <v>3</v>
@@ -946,7 +1272,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G16">
-        <v>2.3549301809667665e-05</v>
+        <v>2.3549301809667665E-5</v>
       </c>
       <c r="H16">
         <v>49.287970038216002</v>
@@ -976,7 +1302,7 @@
         <v>2.76535104008848</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>50</v>
       </c>
@@ -990,13 +1316,13 @@
         <v>1</v>
       </c>
       <c r="E17">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="F17">
         <v>1.1941438923248031</v>
       </c>
       <c r="G17">
-        <v>3.9248836349446107e-05</v>
+        <v>3.9248836349446107E-5</v>
       </c>
       <c r="H17">
         <v>48.332401158804572</v>
@@ -1026,7 +1352,7 @@
         <v>2.8160015228439312</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>50</v>
       </c>
@@ -1046,7 +1372,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G18">
-        <v>2.9436627262084583e-05</v>
+        <v>2.9436627262084583E-5</v>
       </c>
       <c r="H18">
         <v>52.149071043161619</v>
@@ -1076,7 +1402,7 @@
         <v>2.8747904328470359</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>50</v>
       </c>
@@ -1096,7 +1422,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G19">
-        <v>2.3549301809667665e-05</v>
+        <v>2.3549301809667665E-5</v>
       </c>
       <c r="H19">
         <v>50.639567547003061</v>
@@ -1126,7 +1452,7 @@
         <v>2.9189816534267288</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>50</v>
       </c>
@@ -1140,13 +1466,13 @@
         <v>1</v>
       </c>
       <c r="E20">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="F20">
         <v>1.1941438923248031</v>
       </c>
       <c r="G20">
-        <v>3.9248836349446107e-05</v>
+        <v>3.9248836349446107E-5</v>
       </c>
       <c r="H20">
         <v>50.332845200621279</v>
@@ -1170,13 +1496,13 @@
         <v>0.30459233945448183</v>
       </c>
       <c r="O20">
-        <v>0.099844462872482401</v>
+        <v>9.9844462872482401E-2</v>
       </c>
       <c r="P20">
         <v>3.0506683164142587</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>50</v>
       </c>
@@ -1184,7 +1510,7 @@
         <v>7</v>
       </c>
       <c r="C21">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="D21">
         <v>2</v>
@@ -1196,7 +1522,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G21">
-        <v>2.9436627262084583e-05</v>
+        <v>2.9436627262084583E-5</v>
       </c>
       <c r="H21">
         <v>53.867476917194146</v>
@@ -1226,7 +1552,7 @@
         <v>3.0801326066218242</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>50</v>
       </c>
@@ -1246,7 +1572,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G22">
-        <v>2.3549301809667665e-05</v>
+        <v>2.3549301809667665E-5</v>
       </c>
       <c r="H22">
         <v>52.067383414809157</v>
@@ -1276,7 +1602,7 @@
         <v>3.0906864565694772</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>50</v>
       </c>
@@ -1296,7 +1622,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G23">
-        <v>1.9624418174723053e-05</v>
+        <v>1.9624418174723053E-5</v>
       </c>
       <c r="H23">
         <v>49.680861631759385</v>
@@ -1326,7 +1652,7 @@
         <v>3.2782241322745755</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>50</v>
       </c>
@@ -1334,7 +1660,7 @@
         <v>7</v>
       </c>
       <c r="C24">
-        <v>1.6000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="D24">
         <v>3</v>
@@ -1346,7 +1672,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G24">
-        <v>2.3549301809667665e-05</v>
+        <v>2.3549301809667665E-5</v>
       </c>
       <c r="H24">
         <v>53.578051775477064</v>
@@ -1376,7 +1702,7 @@
         <v>3.2838543601050691</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>50</v>
       </c>
@@ -1396,7 +1722,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G25">
-        <v>2.9436627262084583e-05</v>
+        <v>2.9436627262084583E-5</v>
       </c>
       <c r="H25">
         <v>55.702990853870936</v>
@@ -1426,7 +1752,7 @@
         <v>3.3170658840542719</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>50</v>
       </c>
@@ -1440,13 +1766,13 @@
         <v>1</v>
       </c>
       <c r="E26">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="F26">
         <v>1.1941438923248031</v>
       </c>
       <c r="G26">
-        <v>3.9248836349446107e-05</v>
+        <v>3.9248836349446107E-5</v>
       </c>
       <c r="H26">
         <v>52.506032921464296</v>
@@ -1470,13 +1796,13 @@
         <v>0.30459233945448183</v>
       </c>
       <c r="O26">
-        <v>0.091524090966442206</v>
+        <v>9.1524090966442206E-2</v>
       </c>
       <c r="P26">
         <v>3.3280017997246456</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>50</v>
       </c>
@@ -1484,7 +1810,7 @@
         <v>7</v>
       </c>
       <c r="C27">
-        <v>1.8999999999999999</v>
+        <v>1.9</v>
       </c>
       <c r="D27">
         <v>4</v>
@@ -1496,7 +1822,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G27">
-        <v>1.9624418174723053e-05</v>
+        <v>1.9624418174723053E-5</v>
       </c>
       <c r="H27">
         <v>50.963070530609457</v>
@@ -1526,7 +1852,7 @@
         <v>3.4507622444995536</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>50</v>
       </c>
@@ -1546,7 +1872,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G28">
-        <v>2.3549301809667665e-05</v>
+        <v>2.3549301809667665E-5</v>
       </c>
       <c r="H28">
         <v>55.178999692222909</v>
@@ -1576,7 +1902,7 @@
         <v>3.5027779841120741</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>50</v>
       </c>
@@ -1596,7 +1922,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G29">
-        <v>2.9436627262084583e-05</v>
+        <v>2.9436627262084583E-5</v>
       </c>
       <c r="H29">
         <v>57.668006397588655</v>
@@ -1626,7 +1952,7 @@
         <v>3.5934880410587944</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>50</v>
       </c>
@@ -1646,7 +1972,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G30">
-        <v>1.9624418174723053e-05</v>
+        <v>1.9624418174723053E-5</v>
       </c>
       <c r="H30">
         <v>52.313217670193744</v>
@@ -1676,7 +2002,7 @@
         <v>3.6424712580828613</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>50</v>
       </c>
@@ -1690,13 +2016,13 @@
         <v>1</v>
       </c>
       <c r="E31">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="F31">
         <v>1.1941438923248031</v>
       </c>
       <c r="G31">
-        <v>3.9248836349446107e-05</v>
+        <v>3.9248836349446107E-5</v>
       </c>
       <c r="H31">
         <v>54.875349315855573</v>
@@ -1720,13 +2046,13 @@
         <v>0.30459233945448183</v>
       </c>
       <c r="O31">
-        <v>0.083203719060401998</v>
+        <v>8.3203719060401998E-2</v>
       </c>
       <c r="P31">
         <v>3.6608019796971103</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>50</v>
       </c>
@@ -1734,7 +2060,7 @@
         <v>7</v>
       </c>
       <c r="C32">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="D32">
         <v>3</v>
@@ -1746,7 +2072,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G32">
-        <v>2.3549301809667665e-05</v>
+        <v>2.3549301809667665E-5</v>
       </c>
       <c r="H32">
         <v>56.878569272811305</v>
@@ -1776,7 +2102,7 @@
         <v>3.7529764115486515</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>50</v>
       </c>
@@ -1796,7 +2122,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G33">
-        <v>1.9624418174723053e-05</v>
+        <v>1.9624418174723053E-5</v>
       </c>
       <c r="H33">
         <v>53.736849586482727</v>
@@ -1826,7 +2152,7 @@
         <v>3.8567342732642067</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>50</v>
       </c>
@@ -1846,7 +2172,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G34">
-        <v>2.9436627262084583e-05</v>
+        <v>2.9436627262084583E-5</v>
       </c>
       <c r="H34">
         <v>59.776729852323342</v>
@@ -1876,7 +2202,7 @@
         <v>3.9201687720641392</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>50</v>
       </c>
@@ -1896,7 +2222,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G35">
-        <v>2.3549301809667665e-05</v>
+        <v>2.3549301809667665E-5</v>
       </c>
       <c r="H35">
         <v>58.686163069560251</v>
@@ -1926,7 +2252,7 @@
         <v>4.0416669047447016</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>50</v>
       </c>
@@ -1934,19 +2260,19 @@
         <v>7</v>
       </c>
       <c r="C36">
-        <v>0.90000000000000002</v>
+        <v>0.9</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="F36">
         <v>1.1941438923248031</v>
       </c>
       <c r="G36">
-        <v>3.9248836349446107e-05</v>
+        <v>3.9248836349446107E-5</v>
       </c>
       <c r="H36">
         <v>57.46859980747476</v>
@@ -1970,13 +2296,13 @@
         <v>0.30459233945448183</v>
       </c>
       <c r="O36">
-        <v>0.074883347154361804</v>
+        <v>7.4883347154361804E-2</v>
       </c>
       <c r="P36">
         <v>4.0675577552190116</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>50</v>
       </c>
@@ -1984,7 +2310,7 @@
         <v>7</v>
       </c>
       <c r="C37">
-        <v>1.6000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="D37">
         <v>4</v>
@@ -1996,7 +2322,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G37">
-        <v>1.9624418174723053e-05</v>
+        <v>1.9624418174723053E-5</v>
       </c>
       <c r="H37">
         <v>55.240133470971116</v>
@@ -2026,7 +2352,7 @@
         <v>4.0977801653432193</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>50</v>
       </c>
@@ -2040,13 +2366,13 @@
         <v>5</v>
       </c>
       <c r="E38">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="F38">
         <v>1.1941438923248031</v>
       </c>
       <c r="G38">
-        <v>1.6820929864048334e-05</v>
+        <v>1.6820929864048334E-5</v>
       </c>
       <c r="H38">
         <v>50.742640744161037</v>
@@ -2076,7 +2402,7 @@
         <v>4.0984643975933608</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>50</v>
       </c>
@@ -2096,7 +2422,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G39">
-        <v>2.9436627262084583e-05</v>
+        <v>2.9436627262084583E-5</v>
       </c>
       <c r="H39">
         <v>62.045524293327645</v>
@@ -2126,7 +2452,7 @@
         <v>4.3121856492705533</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>50</v>
       </c>
@@ -2134,19 +2460,19 @@
         <v>7</v>
       </c>
       <c r="C40">
-        <v>1.8999999999999999</v>
+        <v>1.9</v>
       </c>
       <c r="D40">
         <v>5</v>
       </c>
       <c r="E40">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="F40">
         <v>1.1941438923248031</v>
       </c>
       <c r="G40">
-        <v>1.6820929864048334e-05</v>
+        <v>1.6820929864048334E-5</v>
       </c>
       <c r="H40">
         <v>52.023921233201676</v>
@@ -2176,7 +2502,7 @@
         <v>4.3141730500982751</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>50</v>
       </c>
@@ -2196,7 +2522,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G41">
-        <v>1.9624418174723053e-05</v>
+        <v>1.9624418174723053E-5</v>
       </c>
       <c r="H41">
         <v>56.829946483118796</v>
@@ -2226,7 +2552,7 @@
         <v>4.3709655096994338</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>50</v>
       </c>
@@ -2246,7 +2572,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G42">
-        <v>2.3549301809667665e-05</v>
+        <v>2.3549301809667665E-5</v>
       </c>
       <c r="H42">
         <v>60.612418114118995</v>
@@ -2276,7 +2602,7 @@
         <v>4.3784724801400925</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>50</v>
       </c>
@@ -2290,13 +2616,13 @@
         <v>5</v>
       </c>
       <c r="E43">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="F43">
         <v>1.1941438923248031</v>
       </c>
       <c r="G43">
-        <v>1.6820929864048334e-05</v>
+        <v>1.6820929864048334E-5</v>
       </c>
       <c r="H43">
         <v>53.37158403292397</v>
@@ -2326,7 +2652,7 @@
         <v>4.5538493306592898</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>50</v>
       </c>
@@ -2334,19 +2660,19 @@
         <v>7</v>
       </c>
       <c r="C44">
-        <v>0.80000000000000004</v>
+        <v>0.8</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="F44">
         <v>1.1941438923248031</v>
       </c>
       <c r="G44">
-        <v>3.9248836349446107e-05</v>
+        <v>3.9248836349446107E-5</v>
       </c>
       <c r="H44">
         <v>60.319106540274724</v>
@@ -2370,13 +2696,13 @@
         <v>0.30459233945448183</v>
       </c>
       <c r="O44">
-        <v>0.066562975248321596</v>
+        <v>6.6562975248321596E-2</v>
       </c>
       <c r="P44">
         <v>4.5760024746213883</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>50</v>
       </c>
@@ -2384,7 +2710,7 @@
         <v>7</v>
       </c>
       <c r="C45">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="D45">
         <v>4</v>
@@ -2396,7 +2722,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G45">
-        <v>1.9624418174723053e-05</v>
+        <v>1.9624418174723053E-5</v>
       </c>
       <c r="H45">
         <v>58.513980942295227</v>
@@ -2426,7 +2752,7 @@
         <v>4.6831773318208221</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>50</v>
       </c>
@@ -2446,7 +2772,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G46">
-        <v>2.3549301809667665e-05</v>
+        <v>2.3549301809667665E-5</v>
       </c>
       <c r="H46">
         <v>62.669415389445717</v>
@@ -2476,7 +2802,7 @@
         <v>4.7765154328801005</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>50</v>
       </c>
@@ -2484,7 +2810,7 @@
         <v>7</v>
       </c>
       <c r="C47">
-        <v>0.90000000000000002</v>
+        <v>0.9</v>
       </c>
       <c r="D47">
         <v>2</v>
@@ -2496,7 +2822,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G47">
-        <v>2.9436627262084583e-05</v>
+        <v>2.9436627262084583E-5</v>
       </c>
       <c r="H47">
         <v>64.493335010215148</v>
@@ -2526,7 +2852,7 @@
         <v>4.7913173880783928</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>50</v>
       </c>
@@ -2540,13 +2866,13 @@
         <v>5</v>
       </c>
       <c r="E48">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="F48">
         <v>1.1941438923248031</v>
       </c>
       <c r="G48">
-        <v>1.6820929864048334e-05</v>
+        <v>1.6820929864048334E-5</v>
       </c>
       <c r="H48">
         <v>54.790925171888269</v>
@@ -2576,7 +2902,7 @@
         <v>4.8217228206980716</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>50</v>
       </c>
@@ -2596,7 +2922,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G49">
-        <v>1.9624418174723053e-05</v>
+        <v>1.9624418174723053E-5</v>
       </c>
       <c r="H49">
         <v>60.300868793703607</v>
@@ -2626,7 +2952,7 @@
         <v>5.0434217419608851</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>50</v>
       </c>
@@ -2634,19 +2960,19 @@
         <v>7</v>
       </c>
       <c r="C50">
-        <v>1.6000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="D50">
         <v>5</v>
       </c>
       <c r="E50">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="F50">
         <v>1.1941438923248031</v>
       </c>
       <c r="G50">
-        <v>1.6820929864048334e-05</v>
+        <v>1.6820929864048334E-5</v>
       </c>
       <c r="H50">
         <v>56.287819431046749</v>
@@ -2676,7 +3002,7 @@
         <v>5.123080496991701</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2684,19 +3010,19 @@
         <v>7</v>
       </c>
       <c r="C51">
-        <v>0.69999999999999996</v>
+        <v>0.7</v>
       </c>
       <c r="D51">
         <v>1</v>
       </c>
       <c r="E51">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="F51">
         <v>1.1941438923248031</v>
       </c>
       <c r="G51">
-        <v>3.9248836349446107e-05</v>
+        <v>3.9248836349446107E-5</v>
       </c>
       <c r="H51">
         <v>63.467147960806479</v>
@@ -2720,13 +3046,13 @@
         <v>0.30459233945448183</v>
       </c>
       <c r="O51">
-        <v>0.058242603342281395</v>
+        <v>5.8242603342281395E-2</v>
       </c>
       <c r="P51">
         <v>5.229717113853015</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2746,7 +3072,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G52">
-        <v>2.3549301809667665e-05</v>
+        <v>2.3549301809667665E-5</v>
       </c>
       <c r="H52">
         <v>64.870933453115896</v>
@@ -2776,7 +3102,7 @@
         <v>5.2541669761681113</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>50</v>
       </c>
@@ -2784,7 +3110,7 @@
         <v>7</v>
       </c>
       <c r="C53">
-        <v>0.80000000000000004</v>
+        <v>0.8</v>
       </c>
       <c r="D53">
         <v>2</v>
@@ -2796,7 +3122,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G53">
-        <v>2.9436627262084583e-05</v>
+        <v>2.9436627262084583E-5</v>
       </c>
       <c r="H53">
         <v>67.142219793409694</v>
@@ -2820,13 +3146,13 @@
         <v>0.48230771197463534</v>
       </c>
       <c r="O53">
-        <v>0.089478097874792981</v>
+        <v>8.9478097874792981E-2</v>
       </c>
       <c r="P53">
         <v>5.3902320615881916</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>50</v>
       </c>
@@ -2846,7 +3172,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G54">
-        <v>1.9624418174723053e-05</v>
+        <v>1.9624418174723053E-5</v>
       </c>
       <c r="H54">
         <v>62.200329598159144</v>
@@ -2876,7 +3202,7 @@
         <v>5.4637068871242933</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>50</v>
       </c>
@@ -2890,13 +3216,13 @@
         <v>5</v>
       </c>
       <c r="E55">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="F55">
         <v>1.1941438923248031</v>
       </c>
       <c r="G55">
-        <v>1.6820929864048334e-05</v>
+        <v>1.6820929864048334E-5</v>
       </c>
       <c r="H55">
         <v>57.868801622182886</v>
@@ -2926,7 +3252,7 @@
         <v>5.4646191967911477</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>50</v>
       </c>
@@ -2934,7 +3260,7 @@
         <v>7</v>
       </c>
       <c r="C56">
-        <v>0.90000000000000002</v>
+        <v>0.9</v>
       </c>
       <c r="D56">
         <v>3</v>
@@ -2946,7 +3272,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G56">
-        <v>2.3549301809667665e-05</v>
+        <v>2.3549301809667665E-5</v>
       </c>
       <c r="H56">
         <v>67.232757464206514</v>
@@ -2976,7 +3302,7 @@
         <v>5.8379633068534575</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>50</v>
       </c>
@@ -2984,19 +3310,19 @@
         <v>7</v>
       </c>
       <c r="C57">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="D57">
         <v>5</v>
       </c>
       <c r="E57">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="F57">
         <v>1.1941438923248031</v>
       </c>
       <c r="G57">
-        <v>1.6820929864048334e-05</v>
+        <v>1.6820929864048334E-5</v>
       </c>
       <c r="H57">
         <v>59.541161959627409</v>
@@ -3026,7 +3352,7 @@
         <v>5.8549491394190873</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>50</v>
       </c>
@@ -3046,7 +3372,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G58">
-        <v>1.9624418174723053e-05</v>
+        <v>1.9624418174723053E-5</v>
       </c>
       <c r="H58">
         <v>64.223347401388665</v>
@@ -3076,7 +3402,7 @@
         <v>5.9604075132265004</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>50</v>
       </c>
@@ -3084,19 +3410,19 @@
         <v>7</v>
       </c>
       <c r="C59">
-        <v>0.59999999999999998</v>
+        <v>0.6</v>
       </c>
       <c r="D59">
         <v>1</v>
       </c>
       <c r="E59">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="F59">
         <v>1.1941438923248031</v>
       </c>
       <c r="G59">
-        <v>3.9248836349446107e-05</v>
+        <v>3.9248836349446107E-5</v>
       </c>
       <c r="H59">
         <v>66.961874011565996</v>
@@ -3120,13 +3446,13 @@
         <v>0.30459233945448183</v>
       </c>
       <c r="O59">
-        <v>0.0499222314362412</v>
+        <v>4.99222314362412E-2</v>
       </c>
       <c r="P59">
         <v>6.1013366328285175</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>50</v>
       </c>
@@ -3134,7 +3460,7 @@
         <v>7</v>
       </c>
       <c r="C60">
-        <v>0.69999999999999996</v>
+        <v>0.7</v>
       </c>
       <c r="D60">
         <v>2</v>
@@ -3146,7 +3472,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G60">
-        <v>2.9436627262084583e-05</v>
+        <v>2.9436627262084583E-5</v>
       </c>
       <c r="H60">
         <v>70.018015498081709</v>
@@ -3170,13 +3496,13 @@
         <v>0.48230771197463534</v>
       </c>
       <c r="O60">
-        <v>0.078293335640443842</v>
+        <v>7.8293335640443842E-2</v>
       </c>
       <c r="P60">
         <v>6.1602652132436484</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>50</v>
       </c>
@@ -3190,13 +3516,13 @@
         <v>5</v>
       </c>
       <c r="E61">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="F61">
         <v>1.1941438923248031</v>
       </c>
       <c r="G61">
-        <v>1.6820929864048334e-05</v>
+        <v>1.6820929864048334E-5</v>
       </c>
       <c r="H61">
         <v>61.313058461082271</v>
@@ -3226,7 +3552,7 @@
         <v>6.3053298424513242</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>50</v>
       </c>
@@ -3246,7 +3572,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G62">
-        <v>1.9624418174723053e-05</v>
+        <v>1.9624418174723053E-5</v>
       </c>
       <c r="H62">
         <v>66.382383278876134</v>
@@ -3276,7 +3602,7 @@
         <v>6.5564482645491511</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>50</v>
       </c>
@@ -3284,7 +3610,7 @@
         <v>7</v>
       </c>
       <c r="C63">
-        <v>0.80000000000000004</v>
+        <v>0.8</v>
       </c>
       <c r="D63">
         <v>3</v>
@@ -3296,7 +3622,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G63">
-        <v>2.3549301809667665e-05</v>
+        <v>2.3549301809667665E-5</v>
       </c>
       <c r="H63">
         <v>69.773058267212974</v>
@@ -3326,7 +3652,7 @@
         <v>6.5677087202101383</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>50</v>
       </c>
@@ -3340,13 +3666,13 @@
         <v>5</v>
       </c>
       <c r="E64">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="F64">
         <v>1.1941438923248031</v>
       </c>
       <c r="G64">
-        <v>1.6820929864048334e-05</v>
+        <v>1.6820929864048334E-5</v>
       </c>
       <c r="H64">
         <v>63.193650033764662</v>
@@ -3376,7 +3702,7 @@
         <v>6.8307739959889355</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>50</v>
       </c>
@@ -3384,7 +3710,7 @@
         <v>7</v>
       </c>
       <c r="C65">
-        <v>0.59999999999999998</v>
+        <v>0.6</v>
       </c>
       <c r="D65">
         <v>2</v>
@@ -3396,7 +3722,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G65">
-        <v>2.9436627262084583e-05</v>
+        <v>2.9436627262084583E-5</v>
       </c>
       <c r="H65">
         <v>73.151183572611757</v>
@@ -3420,13 +3746,13 @@
         <v>0.48230771197463534</v>
       </c>
       <c r="O65">
-        <v>0.067108573406094732</v>
+        <v>6.7108573406094732E-2</v>
       </c>
       <c r="P65">
         <v>7.1869760821175888</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>50</v>
       </c>
@@ -3434,7 +3760,7 @@
         <v>7</v>
       </c>
       <c r="C66">
-        <v>0.90000000000000002</v>
+        <v>0.9</v>
       </c>
       <c r="D66">
         <v>4</v>
@@ -3446,7 +3772,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G66">
-        <v>1.9624418174723053e-05</v>
+        <v>1.9624418174723053E-5</v>
       </c>
       <c r="H66">
         <v>68.69163224358951</v>
@@ -3476,7 +3802,7 @@
         <v>7.2849425161657226</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>50</v>
       </c>
@@ -3490,13 +3816,13 @@
         <v>1</v>
       </c>
       <c r="E67">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="F67">
         <v>1.1941438923248031</v>
       </c>
       <c r="G67">
-        <v>3.9248836349446107e-05</v>
+        <v>3.9248836349446107E-5</v>
       </c>
       <c r="H67">
         <v>70.863890939728307</v>
@@ -3520,13 +3846,13 @@
         <v>0.30459233945448183</v>
       </c>
       <c r="O67">
-        <v>0.041601859530200999</v>
+        <v>4.1601859530200999E-2</v>
       </c>
       <c r="P67">
         <v>7.3216039593942206</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>50</v>
       </c>
@@ -3540,13 +3866,13 @@
         <v>5</v>
       </c>
       <c r="E68">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="F68">
         <v>1.1941438923248031</v>
       </c>
       <c r="G68">
-        <v>1.6820929864048334e-05</v>
+        <v>1.6820929864048334E-5</v>
       </c>
       <c r="H68">
         <v>65.193254827617352</v>
@@ -3576,7 +3902,7 @@
         <v>7.4517534501697469</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>50</v>
       </c>
@@ -3584,7 +3910,7 @@
         <v>7</v>
       </c>
       <c r="C69">
-        <v>0.69999999999999996</v>
+        <v>0.7</v>
       </c>
       <c r="D69">
         <v>3</v>
@@ -3596,7 +3922,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G69">
-        <v>2.3549301809667665e-05</v>
+        <v>2.3549301809667665E-5</v>
       </c>
       <c r="H69">
         <v>72.512860789671876</v>
@@ -3620,13 +3946,13 @@
         <v>0.66384502045343996</v>
       </c>
       <c r="O69">
-        <v>0.0884424717419829</v>
+        <v>8.84424717419829E-2</v>
       </c>
       <c r="P69">
         <v>7.5059528230973029</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>50</v>
       </c>
@@ -3634,7 +3960,7 @@
         <v>7</v>
       </c>
       <c r="C70">
-        <v>0.80000000000000004</v>
+        <v>0.8</v>
       </c>
       <c r="D70">
         <v>4</v>
@@ -3646,7 +3972,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G70">
-        <v>1.9624418174723053e-05</v>
+        <v>1.9624418174723053E-5</v>
       </c>
       <c r="H70">
         <v>71.167335708714333</v>
@@ -3676,7 +4002,7 @@
         <v>8.1955603306864386</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>50</v>
       </c>
@@ -3690,13 +4016,13 @@
         <v>5</v>
       </c>
       <c r="E71">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="F71">
         <v>1.1941438923248031</v>
       </c>
       <c r="G71">
-        <v>1.6820929864048334e-05</v>
+        <v>1.6820929864048334E-5</v>
       </c>
       <c r="H71">
         <v>67.323539635053848</v>
@@ -3726,7 +4052,7 @@
         <v>8.1969287951867216</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>50</v>
       </c>
@@ -3746,7 +4072,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G72">
-        <v>2.9436627262084583e-05</v>
+        <v>2.9436627262084583E-5</v>
       </c>
       <c r="H72">
         <v>76.577893235749713</v>
@@ -3770,13 +4096,13 @@
         <v>0.48230771197463534</v>
       </c>
       <c r="O72">
-        <v>0.055923811171745608</v>
+        <v>5.5923811171745608E-2</v>
       </c>
       <c r="P72">
         <v>8.6243712985411065</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>50</v>
       </c>
@@ -3784,7 +4110,7 @@
         <v>7</v>
       </c>
       <c r="C73">
-        <v>0.59999999999999998</v>
+        <v>0.6</v>
       </c>
       <c r="D73">
         <v>3</v>
@@ -3796,7 +4122,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G73">
-        <v>2.3549301809667665e-05</v>
+        <v>2.3549301809667665E-5</v>
       </c>
       <c r="H73">
         <v>75.476627306678637</v>
@@ -3820,13 +4146,13 @@
         <v>0.66384502045343996</v>
       </c>
       <c r="O73">
-        <v>0.075807832921699639</v>
+        <v>7.5807832921699639E-2</v>
       </c>
       <c r="P73">
         <v>8.756944960280185</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>50</v>
       </c>
@@ -3834,19 +4160,19 @@
         <v>7</v>
       </c>
       <c r="C74">
-        <v>0.90000000000000002</v>
+        <v>0.9</v>
       </c>
       <c r="D74">
         <v>5</v>
       </c>
       <c r="E74">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="F74">
         <v>1.1941438923248031</v>
       </c>
       <c r="G74">
-        <v>1.6820929864048334e-05</v>
+        <v>1.6820929864048334E-5</v>
       </c>
       <c r="H74">
         <v>69.597747678561888</v>
@@ -3876,7 +4202,7 @@
         <v>9.1076986613185795</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>50</v>
       </c>
@@ -3884,19 +4210,19 @@
         <v>7</v>
       </c>
       <c r="C75">
-        <v>0.40000000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="D75">
         <v>1</v>
       </c>
       <c r="E75">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="F75">
         <v>1.1941438923248031</v>
       </c>
       <c r="G75">
-        <v>3.9248836349446107e-05</v>
+        <v>3.9248836349446107E-5</v>
       </c>
       <c r="H75">
         <v>75.248805762426827</v>
@@ -3920,13 +4246,13 @@
         <v>0.30459233945448183</v>
       </c>
       <c r="O75">
-        <v>0.033281487624160798</v>
+        <v>3.3281487624160798E-2</v>
       </c>
       <c r="P75">
         <v>9.1520049492427766</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>50</v>
       </c>
@@ -3934,7 +4260,7 @@
         <v>7</v>
       </c>
       <c r="C76">
-        <v>0.69999999999999996</v>
+        <v>0.7</v>
       </c>
       <c r="D76">
         <v>4</v>
@@ -3946,7 +4272,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G76">
-        <v>1.9624418174723053e-05</v>
+        <v>1.9624418174723053E-5</v>
       </c>
       <c r="H76">
         <v>73.828164045159411</v>
@@ -3970,13 +4296,13 @@
         <v>0.88579627948284834</v>
       </c>
       <c r="O76">
-        <v>0.09457214800132821</v>
+        <v>9.457214800132821E-2</v>
       </c>
       <c r="P76">
         <v>9.3663546636416442</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>50</v>
       </c>
@@ -3984,19 +4310,19 @@
         <v>7</v>
       </c>
       <c r="C77">
-        <v>0.80000000000000004</v>
+        <v>0.8</v>
       </c>
       <c r="D77">
         <v>5</v>
       </c>
       <c r="E77">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="F77">
         <v>1.1941438923248031</v>
       </c>
       <c r="G77">
-        <v>1.6820929864048334e-05</v>
+        <v>1.6820929864048334E-5</v>
       </c>
       <c r="H77">
         <v>72.030974180787766</v>
@@ -4026,7 +4352,7 @@
         <v>10.246160993983402</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>50</v>
       </c>
@@ -4046,7 +4372,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G78">
-        <v>2.3549301809667665e-05</v>
+        <v>2.3549301809667665E-5</v>
       </c>
       <c r="H78">
         <v>78.692989836881281</v>
@@ -4070,13 +4396,13 @@
         <v>0.66384502045343996</v>
       </c>
       <c r="O78">
-        <v>0.063173194101416363</v>
+        <v>6.3173194101416363E-2</v>
       </c>
       <c r="P78">
         <v>10.508333952336223</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>50</v>
       </c>
@@ -4084,7 +4410,7 @@
         <v>7</v>
       </c>
       <c r="C79">
-        <v>0.40000000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="D79">
         <v>2</v>
@@ -4096,7 +4422,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G79">
-        <v>2.9436627262084583e-05</v>
+        <v>2.9436627262084583E-5</v>
       </c>
       <c r="H79">
         <v>80.341424059580504</v>
@@ -4120,13 +4446,13 @@
         <v>0.48230771197463534</v>
       </c>
       <c r="O79">
-        <v>0.04473904893739649</v>
+        <v>4.473904893739649E-2</v>
       </c>
       <c r="P79">
         <v>10.780464123176383</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>50</v>
       </c>
@@ -4134,7 +4460,7 @@
         <v>7</v>
       </c>
       <c r="C80">
-        <v>0.59999999999999998</v>
+        <v>0.6</v>
       </c>
       <c r="D80">
         <v>4</v>
@@ -4146,7 +4472,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G80">
-        <v>1.9624418174723053e-05</v>
+        <v>1.9624418174723053E-5</v>
       </c>
       <c r="H80">
         <v>76.695688291455937</v>
@@ -4170,13 +4496,13 @@
         <v>0.88579627948284834</v>
       </c>
       <c r="O80">
-        <v>0.081061841143995603</v>
+        <v>8.1061841143995603E-2</v>
       </c>
       <c r="P80">
         <v>10.927413774248587</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>50</v>
       </c>
@@ -4184,19 +4510,19 @@
         <v>7</v>
       </c>
       <c r="C81">
-        <v>0.69999999999999996</v>
+        <v>0.7</v>
       </c>
       <c r="D81">
         <v>5</v>
       </c>
       <c r="E81">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="F81">
         <v>1.1941438923248031</v>
       </c>
       <c r="G81">
-        <v>1.6820929864048334e-05</v>
+        <v>1.6820929864048334E-5</v>
       </c>
       <c r="H81">
         <v>74.640501834497826</v>
@@ -4220,13 +4546,13 @@
         <v>1.1554798919812506</v>
       </c>
       <c r="O81">
-        <v>0.098675485001385871</v>
+        <v>9.8675485001385871E-2</v>
       </c>
       <c r="P81">
         <v>11.709898278838175</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>50</v>
       </c>
@@ -4234,19 +4560,19 @@
         <v>7</v>
       </c>
       <c r="C82">
-        <v>0.29999999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="D82">
         <v>1</v>
       </c>
       <c r="E82">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="F82">
         <v>1.1941438923248031</v>
       </c>
       <c r="G82">
-        <v>3.9248836349446107e-05</v>
+        <v>3.9248836349446107E-5</v>
       </c>
       <c r="H82">
         <v>80.212173477314138</v>
@@ -4270,13 +4596,13 @@
         <v>0.30459233945448183</v>
       </c>
       <c r="O82">
-        <v>0.0249611157181206</v>
+        <v>2.49611157181206E-2</v>
       </c>
       <c r="P82">
         <v>12.202673265657035</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>50</v>
       </c>
@@ -4296,7 +4622,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G83">
-        <v>1.9624418174723053e-05</v>
+        <v>1.9624418174723053E-5</v>
       </c>
       <c r="H83">
         <v>79.794966234630223</v>
@@ -4320,13 +4646,13 @@
         <v>0.88579627948284834</v>
       </c>
       <c r="O83">
-        <v>0.067551534286663009</v>
+        <v>6.7551534286663009E-2</v>
       </c>
       <c r="P83">
         <v>13.112896529098302</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>50</v>
       </c>
@@ -4334,7 +4660,7 @@
         <v>7</v>
       </c>
       <c r="C84">
-        <v>0.40000000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="D84">
         <v>3</v>
@@ -4346,7 +4672,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G84">
-        <v>2.3549301809667665e-05</v>
+        <v>2.3549301809667665E-5</v>
       </c>
       <c r="H84">
         <v>82.195678135684176</v>
@@ -4370,13 +4696,13 @@
         <v>0.66384502045343996</v>
       </c>
       <c r="O84">
-        <v>0.050538555281133095</v>
+        <v>5.0538555281133095E-2</v>
       </c>
       <c r="P84">
         <v>13.135417440420277</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>50</v>
       </c>
@@ -4384,19 +4710,19 @@
         <v>7</v>
       </c>
       <c r="C85">
-        <v>0.59999999999999998</v>
+        <v>0.6</v>
       </c>
       <c r="D85">
         <v>5</v>
       </c>
       <c r="E85">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="F85">
         <v>1.1941438923248031</v>
       </c>
       <c r="G85">
-        <v>1.6820929864048334e-05</v>
+        <v>1.6820929864048334E-5</v>
       </c>
       <c r="H85">
         <v>77.446211933724058</v>
@@ -4420,13 +4746,13 @@
         <v>1.1554798919812506</v>
       </c>
       <c r="O85">
-        <v>0.084578987144045034</v>
+        <v>8.4578987144045034E-2</v>
       </c>
       <c r="P85">
         <v>13.661547991977871</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>50</v>
       </c>
@@ -4434,7 +4760,7 @@
         <v>7</v>
       </c>
       <c r="C86">
-        <v>0.29999999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="D86">
         <v>2</v>
@@ -4446,7 +4772,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G86">
-        <v>2.9436627262084583e-05</v>
+        <v>2.9436627262084583E-5</v>
       </c>
       <c r="H86">
         <v>84.494003521420296</v>
@@ -4470,13 +4796,13 @@
         <v>0.48230771197463534</v>
       </c>
       <c r="O86">
-        <v>0.033554286703047366</v>
+        <v>3.3554286703047366E-2</v>
       </c>
       <c r="P86">
         <v>14.373952164235178</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>50</v>
       </c>
@@ -4484,7 +4810,7 @@
         <v>7</v>
       </c>
       <c r="C87">
-        <v>0.40000000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="D87">
         <v>4</v>
@@ -4496,7 +4822,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G87">
-        <v>1.9624418174723053e-05</v>
+        <v>1.9624418174723053E-5</v>
       </c>
       <c r="H87">
         <v>83.155276576629106</v>
@@ -4520,13 +4846,13 @@
         <v>0.88579627948284834</v>
       </c>
       <c r="O87">
-        <v>0.054041227429330409</v>
+        <v>5.4041227429330409E-2</v>
       </c>
       <c r="P87">
         <v>16.391120661372877</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>50</v>
       </c>
@@ -4540,13 +4866,13 @@
         <v>5</v>
       </c>
       <c r="E88">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="F88">
         <v>1.1941438923248031</v>
       </c>
       <c r="G88">
-        <v>1.6820929864048334e-05</v>
+        <v>1.6820929864048334E-5</v>
       </c>
       <c r="H88">
         <v>80.471091852218663</v>
@@ -4570,13 +4896,13 @@
         <v>1.1554798919812506</v>
       </c>
       <c r="O88">
-        <v>0.070482489286704197</v>
+        <v>7.0482489286704197E-2</v>
       </c>
       <c r="P88">
         <v>16.393857590373443</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>50</v>
       </c>
@@ -4584,7 +4910,7 @@
         <v>7</v>
       </c>
       <c r="C89">
-        <v>0.29999999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="D89">
         <v>3</v>
@@ -4596,7 +4922,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G89">
-        <v>2.3549301809667665e-05</v>
+        <v>2.3549301809667665E-5</v>
       </c>
       <c r="H89">
         <v>86.024707067989112</v>
@@ -4620,13 +4946,13 @@
         <v>0.66384502045343996</v>
       </c>
       <c r="O89">
-        <v>0.037903916460849819</v>
+        <v>3.7903916460849819E-2</v>
       </c>
       <c r="P89">
         <v>17.51388992056037</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>50</v>
       </c>
@@ -4634,19 +4960,19 @@
         <v>7</v>
       </c>
       <c r="C90">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="D90">
         <v>1</v>
       </c>
       <c r="E90">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="F90">
         <v>1.1941438923248031</v>
       </c>
       <c r="G90">
-        <v>3.9248836349446107e-05</v>
+        <v>3.9248836349446107E-5</v>
       </c>
       <c r="H90">
         <v>85.876540424973442</v>
@@ -4670,13 +4996,13 @@
         <v>0.30459233945448183</v>
       </c>
       <c r="O90">
-        <v>0.016640743812080399</v>
+        <v>1.6640743812080399E-2</v>
       </c>
       <c r="P90">
         <v>18.304009898485553</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>50</v>
       </c>
@@ -4684,19 +5010,19 @@
         <v>7</v>
       </c>
       <c r="C91">
-        <v>0.40000000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="D91">
         <v>5</v>
       </c>
       <c r="E91">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="F91">
         <v>1.1941438923248031</v>
       </c>
       <c r="G91">
-        <v>1.6820929864048334e-05</v>
+        <v>1.6820929864048334E-5</v>
       </c>
       <c r="H91">
         <v>83.74186628169673</v>
@@ -4720,13 +5046,13 @@
         <v>1.1554798919812506</v>
       </c>
       <c r="O91">
-        <v>0.056385991429363361</v>
+        <v>5.6385991429363361E-2</v>
       </c>
       <c r="P91">
         <v>20.492321987966804</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>50</v>
       </c>
@@ -4734,7 +5060,7 @@
         <v>7</v>
       </c>
       <c r="C92">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="D92">
         <v>2</v>
@@ -4746,7 +5072,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G92">
-        <v>2.9436627262084583e-05</v>
+        <v>2.9436627262084583E-5</v>
       </c>
       <c r="H92">
         <v>89.099245476777</v>
@@ -4770,13 +5096,13 @@
         <v>0.48230771197463534</v>
       </c>
       <c r="O92">
-        <v>0.022369524468698245</v>
+        <v>2.2369524468698245E-2</v>
       </c>
       <c r="P92">
         <v>21.560928246352766</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>50</v>
       </c>
@@ -4784,7 +5110,7 @@
         <v>7</v>
       </c>
       <c r="C93">
-        <v>0.29999999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="D93">
         <v>4</v>
@@ -4796,7 +5122,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G93">
-        <v>1.9624418174723053e-05</v>
+        <v>1.9624418174723053E-5</v>
       </c>
       <c r="H93">
         <v>86.811046758478867</v>
@@ -4820,13 +5146,13 @@
         <v>0.88579627948284834</v>
       </c>
       <c r="O93">
-        <v>0.040530920571997801</v>
+        <v>4.0530920571997801E-2</v>
       </c>
       <c r="P93">
         <v>21.854827548497173</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>50</v>
       </c>
@@ -4834,7 +5160,7 @@
         <v>7</v>
       </c>
       <c r="C94">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="D94">
         <v>3</v>
@@ -4846,7 +5172,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G94">
-        <v>2.3549301809667665e-05</v>
+        <v>2.3549301809667665E-5</v>
       </c>
       <c r="H94">
         <v>90.227912074260814</v>
@@ -4870,13 +5196,13 @@
         <v>0.66384502045343996</v>
       </c>
       <c r="O94">
-        <v>0.025269277640566547</v>
+        <v>2.5269277640566547E-2</v>
       </c>
       <c r="P94">
         <v>26.270834880840553</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>50</v>
       </c>
@@ -4884,19 +5210,19 @@
         <v>7</v>
       </c>
       <c r="C95">
-        <v>0.29999999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="D95">
         <v>5</v>
       </c>
       <c r="E95">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="F95">
         <v>1.1941438923248031</v>
       </c>
       <c r="G95">
-        <v>1.6820929864048334e-05</v>
+        <v>1.6820929864048334E-5</v>
       </c>
       <c r="H95">
         <v>87.289788933505264</v>
@@ -4920,13 +5246,13 @@
         <v>1.1554798919812506</v>
       </c>
       <c r="O95">
-        <v>0.042289493572022517</v>
+        <v>4.2289493572022517E-2</v>
       </c>
       <c r="P95">
         <v>27.323095983955742</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>50</v>
       </c>
@@ -4934,7 +5260,7 @@
         <v>7</v>
       </c>
       <c r="C96">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="D96">
         <v>4</v>
@@ -4946,7 +5272,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G96">
-        <v>1.9624418174723053e-05</v>
+        <v>1.9624418174723053E-5</v>
       </c>
       <c r="H96">
         <v>90.803036779383547</v>
@@ -4970,13 +5296,13 @@
         <v>0.88579627948284834</v>
       </c>
       <c r="O96">
-        <v>0.027020613714665204</v>
+        <v>2.7020613714665204E-2</v>
       </c>
       <c r="P96">
         <v>32.782241322745755</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>50</v>
       </c>
@@ -4984,19 +5310,19 @@
         <v>7</v>
       </c>
       <c r="C97">
-        <v>0.10000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="D97">
         <v>1</v>
       </c>
       <c r="E97">
-        <v>3.6000000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="F97">
         <v>1.1941438923248031</v>
       </c>
       <c r="G97">
-        <v>3.9248836349446107e-05</v>
+        <v>3.9248836349446107E-5</v>
       </c>
       <c r="H97">
         <v>92.401698706713702</v>
@@ -5020,13 +5346,13 @@
         <v>0.30459233945448183</v>
       </c>
       <c r="O97">
-        <v>0.0083203719060401995</v>
+        <v>8.3203719060401995E-3</v>
       </c>
       <c r="P97">
         <v>36.608019796971107</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>50</v>
       </c>
@@ -5034,19 +5360,19 @@
         <v>7</v>
       </c>
       <c r="C98">
-        <v>0.20000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="D98">
         <v>5</v>
       </c>
       <c r="E98">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="F98">
         <v>1.1941438923248031</v>
       </c>
       <c r="G98">
-        <v>1.6820929864048334e-05</v>
+        <v>1.6820929864048334E-5</v>
       </c>
       <c r="H98">
         <v>91.151644398028637</v>
@@ -5070,13 +5396,13 @@
         <v>1.1554798919812506</v>
       </c>
       <c r="O98">
-        <v>0.02819299571468168</v>
+        <v>2.819299571468168E-2</v>
       </c>
       <c r="P98">
         <v>40.984643975933608</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>50</v>
       </c>
@@ -5084,7 +5410,7 @@
         <v>7</v>
       </c>
       <c r="C99">
-        <v>0.10000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="D99">
         <v>2</v>
@@ -5096,7 +5422,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G99">
-        <v>2.9436627262084583e-05</v>
+        <v>2.9436627262084583E-5</v>
       </c>
       <c r="H99">
         <v>94.235432036897407</v>
@@ -5120,13 +5446,13 @@
         <v>0.48230771197463534</v>
       </c>
       <c r="O99">
-        <v>0.011184762234349123</v>
+        <v>1.1184762234349123E-2</v>
       </c>
       <c r="P99">
         <v>43.121856492705533</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>50</v>
       </c>
@@ -5134,7 +5460,7 @@
         <v>7</v>
       </c>
       <c r="C100">
-        <v>0.10000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="D100">
         <v>3</v>
@@ -5146,7 +5472,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G100">
-        <v>2.3549301809667665e-05</v>
+        <v>2.3549301809667665E-5</v>
       </c>
       <c r="H100">
         <v>94.862957901822327</v>
@@ -5170,13 +5496,13 @@
         <v>0.66384502045343996</v>
       </c>
       <c r="O100">
-        <v>0.012634638820283274</v>
+        <v>1.2634638820283274E-2</v>
       </c>
       <c r="P100">
         <v>52.541669761681106</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>50</v>
       </c>
@@ -5184,7 +5510,7 @@
         <v>7</v>
       </c>
       <c r="C101">
-        <v>0.10000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="D101">
         <v>4</v>
@@ -5196,7 +5522,7 @@
         <v>1.1941438923248031</v>
       </c>
       <c r="G101">
-        <v>1.9624418174723053e-05</v>
+        <v>1.9624418174723053E-5</v>
       </c>
       <c r="H101">
         <v>95.179865385868837</v>
@@ -5220,13 +5546,13 @@
         <v>0.88579627948284834</v>
       </c>
       <c r="O101">
-        <v>0.013510306857332602</v>
+        <v>1.3510306857332602E-2</v>
       </c>
       <c r="P101">
         <v>65.564482645491509</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>50</v>
       </c>
@@ -5234,19 +5560,19 @@
         <v>7</v>
       </c>
       <c r="C102">
-        <v>0.10000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="D102">
         <v>5</v>
       </c>
       <c r="E102">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="F102">
         <v>1.1941438923248031</v>
       </c>
       <c r="G102">
-        <v>1.6820929864048334e-05</v>
+        <v>1.6820929864048334E-5</v>
       </c>
       <c r="H102">
         <v>95.371028258827451</v>
@@ -5270,28 +5596,37 @@
         <v>1.1554798919812506</v>
       </c>
       <c r="O102">
-        <v>0.01409649785734084</v>
+        <v>1.409649785734084E-2</v>
       </c>
       <c r="P102">
         <v>81.969287951867216</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>